<commit_message>
Massively sped-up ratios function using multiprocessing
</commit_message>
<xml_diff>
--- a/inputs/transactions_5Y-Prices.xlsx
+++ b/inputs/transactions_5Y-Prices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jackson\PycharmProjects\ic-portfolio\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF8AC4D-B6D3-48D3-9DDB-52D2E519F199}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC469E60-A2F8-4EC1-84AE-303BCD628503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{E9F682BB-0E03-4401-9B9F-39DD7E3E0213}"/>
+    <workbookView xWindow="1470" yWindow="4178" windowWidth="21600" windowHeight="11422" xr2:uid="{E9F682BB-0E03-4401-9B9F-39DD7E3E0213}"/>
   </bookViews>
   <sheets>
     <sheet name="Transactions" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="130">
   <si>
     <t>Action</t>
   </si>
@@ -391,17 +391,48 @@
   </si>
   <si>
     <t>aqn</t>
+  </si>
+  <si>
+    <t>nomd</t>
+  </si>
+  <si>
+    <t>msm</t>
+  </si>
+  <si>
+    <t>dea</t>
+  </si>
+  <si>
+    <t>vmd</t>
+  </si>
+  <si>
+    <t>xlu</t>
+  </si>
+  <si>
+    <t>nni</t>
+  </si>
+  <si>
+    <t>xlc</t>
+  </si>
+  <si>
+    <t>qts</t>
+  </si>
+  <si>
+    <t>unh</t>
+  </si>
+  <si>
+    <t>shyd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,13 +440,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -430,11 +479,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,10 +539,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F62D69AE-DE8A-48F4-B792-FC33582B21AA}" name="Table1" displayName="Table1" ref="A1:F215" totalsRowShown="0">
-  <autoFilter ref="A1:F215" xr:uid="{668E02C6-58B8-4B43-989C-07CB4D4C7424}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F1048571">
-    <sortCondition ref="E1:E1048571"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F62D69AE-DE8A-48F4-B792-FC33582B21AA}" name="Table1" displayName="Table1" ref="A1:F253" totalsRowShown="0">
+  <autoFilter ref="A1:F253" xr:uid="{668E02C6-58B8-4B43-989C-07CB4D4C7424}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F1048572">
+    <sortCondition ref="E1:E1048572"/>
   </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D07F04AB-82CE-4026-AAE4-054084E1418D}" name="Action"/>
@@ -774,10 +853,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067709ED-A958-4B20-93E3-10BACD7AB236}">
-  <dimension ref="A1:F215"/>
+  <dimension ref="A1:F253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="A216" sqref="A216"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1880,7 +1959,7 @@
         <v>162.12</v>
       </c>
       <c r="D55">
-        <v>164</v>
+        <v>422</v>
       </c>
       <c r="E55" s="3">
         <v>43199</v>
@@ -3980,7 +4059,7 @@
         <v>44.849499999999999</v>
       </c>
       <c r="D160">
-        <v>304</v>
+        <v>455.61700000000002</v>
       </c>
       <c r="E160" s="3">
         <v>43936</v>
@@ -4780,7 +4859,7 @@
         <v>54.45</v>
       </c>
       <c r="D200">
-        <v>93</v>
+        <v>139.38300000000001</v>
       </c>
       <c r="E200" s="3">
         <v>44120</v>
@@ -5087,6 +5166,766 @@
       </c>
       <c r="F215" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A216" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B216" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C216" s="8">
+        <v>55.01</v>
+      </c>
+      <c r="D216" s="9">
+        <v>380</v>
+      </c>
+      <c r="E216" s="11">
+        <v>44236</v>
+      </c>
+      <c r="F216" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A217" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B217" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C217" s="8">
+        <v>136.75</v>
+      </c>
+      <c r="D217" s="9">
+        <v>392</v>
+      </c>
+      <c r="E217" s="11">
+        <v>44236</v>
+      </c>
+      <c r="F217" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A218" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B218" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C218" s="8">
+        <v>65.989999999999995</v>
+      </c>
+      <c r="D218" s="9">
+        <v>270</v>
+      </c>
+      <c r="E218" s="11">
+        <v>44236</v>
+      </c>
+      <c r="F218" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A219" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B219" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C219" s="8">
+        <v>172.44</v>
+      </c>
+      <c r="D219" s="9">
+        <v>103</v>
+      </c>
+      <c r="E219" s="11">
+        <v>44236</v>
+      </c>
+      <c r="F219" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A220" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B220" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C220" s="8">
+        <v>115.85</v>
+      </c>
+      <c r="D220" s="9">
+        <v>182</v>
+      </c>
+      <c r="E220" s="11">
+        <v>44236</v>
+      </c>
+      <c r="F220" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A221" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B221" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C221" s="8">
+        <v>116.95</v>
+      </c>
+      <c r="D221" s="9">
+        <v>213</v>
+      </c>
+      <c r="E221" s="11">
+        <v>44236</v>
+      </c>
+      <c r="F221" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A222" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B222" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C222" s="8">
+        <v>3250.03</v>
+      </c>
+      <c r="D222" s="9">
+        <v>4</v>
+      </c>
+      <c r="E222" s="11">
+        <v>44239</v>
+      </c>
+      <c r="F222" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A223" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B223" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C223" s="8">
+        <v>110.36</v>
+      </c>
+      <c r="D223" s="9">
+        <v>265</v>
+      </c>
+      <c r="E223" s="11">
+        <v>44239</v>
+      </c>
+      <c r="F223" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A224" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B224" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C224" s="8">
+        <v>243.8</v>
+      </c>
+      <c r="D224" s="9">
+        <v>36</v>
+      </c>
+      <c r="E224" s="11">
+        <v>44239</v>
+      </c>
+      <c r="F224" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A225" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B225" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C225" s="8">
+        <v>169.47</v>
+      </c>
+      <c r="D225" s="9">
+        <v>102</v>
+      </c>
+      <c r="E225" s="11">
+        <v>44239</v>
+      </c>
+      <c r="F225" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A226" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B226" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C226" s="8">
+        <v>31.38</v>
+      </c>
+      <c r="D226" s="9">
+        <v>588</v>
+      </c>
+      <c r="E226" s="11">
+        <v>44239</v>
+      </c>
+      <c r="F226" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A227" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B227" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C227" s="8">
+        <v>64.83</v>
+      </c>
+      <c r="D227" s="9">
+        <v>254</v>
+      </c>
+      <c r="E227" s="11">
+        <v>44249</v>
+      </c>
+      <c r="F227" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A228" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B228" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C228" s="8">
+        <v>25.53</v>
+      </c>
+      <c r="D228" s="9">
+        <v>645</v>
+      </c>
+      <c r="E228" s="11">
+        <v>44249</v>
+      </c>
+      <c r="F228" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A229" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B229" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C229" s="8">
+        <v>42.02</v>
+      </c>
+      <c r="D229" s="9">
+        <v>338</v>
+      </c>
+      <c r="E229" s="11">
+        <v>44253</v>
+      </c>
+      <c r="F229" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A230" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B230" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C230" s="9">
+        <v>86.52</v>
+      </c>
+      <c r="D230" s="9">
+        <v>304</v>
+      </c>
+      <c r="E230" s="11">
+        <v>44253</v>
+      </c>
+      <c r="F230" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A231" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B231" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C231" s="9">
+        <v>22.29</v>
+      </c>
+      <c r="D231" s="9">
+        <v>591</v>
+      </c>
+      <c r="E231" s="11">
+        <v>44253</v>
+      </c>
+      <c r="F231" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A232" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B232" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C232" s="9">
+        <v>91.5</v>
+      </c>
+      <c r="D232" s="9">
+        <v>334</v>
+      </c>
+      <c r="E232" s="11">
+        <v>44253</v>
+      </c>
+      <c r="F232" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A233" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B233" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C233" s="9">
+        <v>48.44</v>
+      </c>
+      <c r="D233" s="9">
+        <v>557</v>
+      </c>
+      <c r="E233" s="11">
+        <v>44253</v>
+      </c>
+      <c r="F233" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A234" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B234" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C234" s="9">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="D234" s="9">
+        <v>1000</v>
+      </c>
+      <c r="E234" s="11">
+        <v>44278</v>
+      </c>
+      <c r="F234" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A235" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B235" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C235" s="9">
+        <v>9.16</v>
+      </c>
+      <c r="D235" s="9">
+        <v>1945</v>
+      </c>
+      <c r="E235" s="11">
+        <v>44278</v>
+      </c>
+      <c r="F235" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A236" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B236" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C236" s="9">
+        <v>115.37</v>
+      </c>
+      <c r="D236" s="9">
+        <v>229</v>
+      </c>
+      <c r="E236" s="11">
+        <v>44278</v>
+      </c>
+      <c r="F236" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A237" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B237" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C237" s="9">
+        <v>26.11</v>
+      </c>
+      <c r="D237" s="9">
+        <v>1416</v>
+      </c>
+      <c r="E237" s="11">
+        <v>44285</v>
+      </c>
+      <c r="F237" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A238" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B238" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C238" s="13">
+        <v>63.59</v>
+      </c>
+      <c r="D238" s="9">
+        <v>442</v>
+      </c>
+      <c r="E238" s="11">
+        <v>44285</v>
+      </c>
+      <c r="F238" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A239" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C239" s="9">
+        <v>34.79</v>
+      </c>
+      <c r="D239" s="9">
+        <v>588</v>
+      </c>
+      <c r="E239" s="11">
+        <v>44292</v>
+      </c>
+      <c r="F239" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A240" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B240" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C240" s="9">
+        <v>74.69</v>
+      </c>
+      <c r="D240" s="9">
+        <v>369</v>
+      </c>
+      <c r="E240" s="11">
+        <v>44292</v>
+      </c>
+      <c r="F240" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A241" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B241" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C241" s="9">
+        <v>258.52</v>
+      </c>
+      <c r="D241" s="9">
+        <v>95</v>
+      </c>
+      <c r="E241" s="11">
+        <v>44299</v>
+      </c>
+      <c r="F241" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A242" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B242" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C242" s="9">
+        <v>76.75</v>
+      </c>
+      <c r="D242" s="9">
+        <v>451</v>
+      </c>
+      <c r="E242" s="11">
+        <v>44299</v>
+      </c>
+      <c r="F242" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A243" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B243" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C243" s="10">
+        <v>215.09</v>
+      </c>
+      <c r="D243" s="10">
+        <v>258</v>
+      </c>
+      <c r="E243" s="12">
+        <v>44305</v>
+      </c>
+      <c r="F243" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A244" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B244" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C244" s="10">
+        <v>178.20500000000001</v>
+      </c>
+      <c r="D244" s="10">
+        <v>308</v>
+      </c>
+      <c r="E244" s="12">
+        <v>44305</v>
+      </c>
+      <c r="F244" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A245" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B245" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C245" s="10">
+        <v>252.93</v>
+      </c>
+      <c r="D245" s="10">
+        <v>48</v>
+      </c>
+      <c r="E245" s="12">
+        <v>44313</v>
+      </c>
+      <c r="F245" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A246" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B246" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C246" s="10">
+        <v>65.180000000000007</v>
+      </c>
+      <c r="D246" s="10">
+        <v>215</v>
+      </c>
+      <c r="E246" s="12">
+        <v>44313</v>
+      </c>
+      <c r="F246" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A247" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B247" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C247" s="10">
+        <v>48.18</v>
+      </c>
+      <c r="D247" s="10">
+        <v>557</v>
+      </c>
+      <c r="E247" s="12">
+        <v>44313</v>
+      </c>
+      <c r="F247" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A248" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B248" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C248" s="10">
+        <v>58.84</v>
+      </c>
+      <c r="D248" s="10">
+        <v>544</v>
+      </c>
+      <c r="E248" s="12">
+        <v>44313</v>
+      </c>
+      <c r="F248" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A249" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B249" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C249" s="10">
+        <v>122.78</v>
+      </c>
+      <c r="D249" s="10">
+        <v>229</v>
+      </c>
+      <c r="E249" s="12">
+        <v>44313</v>
+      </c>
+      <c r="F249" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A250" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B250" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C250" s="10">
+        <v>122.78</v>
+      </c>
+      <c r="D250" s="10">
+        <v>53</v>
+      </c>
+      <c r="E250" s="12">
+        <v>44313</v>
+      </c>
+      <c r="F250" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A251" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B251" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C251" s="10">
+        <v>395.92</v>
+      </c>
+      <c r="D251" s="10">
+        <v>71</v>
+      </c>
+      <c r="E251" s="12">
+        <v>44313</v>
+      </c>
+      <c r="F251" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A252" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B252" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C252" s="10">
+        <v>114.45</v>
+      </c>
+      <c r="D252" s="10">
+        <v>157</v>
+      </c>
+      <c r="E252" s="12">
+        <v>44313</v>
+      </c>
+      <c r="F252" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A253" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B253" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C253" s="10">
+        <v>25.16</v>
+      </c>
+      <c r="D253" s="10">
+        <v>1433</v>
+      </c>
+      <c r="E253" s="12">
+        <v>44313</v>
+      </c>
+      <c r="F253" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>